<commit_message>
alpha support and more
</commit_message>
<xml_diff>
--- a/ops.xlsx
+++ b/ops.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Atlas\Documents\Scratch\Image Format 2\image_format\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1481E518-0A48-4897-A462-130CE3A45773}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BA6590A-D763-445F-ACF7-44F34DB8A26E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{82B26506-029A-4AF7-9821-B95842BC404D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="2" xr2:uid="{82B26506-029A-4AF7-9821-B95842BC404D}"/>
   </bookViews>
   <sheets>
     <sheet name="INFO" sheetId="3" r:id="rId1"/>
@@ -843,7 +843,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D621977D-9180-48C3-AE56-C4DE55E27DCB}">
   <dimension ref="A1:I96"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
@@ -3262,8 +3262,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BFE32E1-971E-421F-948C-724DF4FBA657}">
   <dimension ref="A1:I96"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3331,7 +3331,7 @@
       </c>
       <c r="I2" s="1" t="str">
         <f>_xlfn.CONCAT(H2:H95)</f>
-        <v>["raw",0,1],["raw",1,1],["raw",2,0],["copy_prev",0,0],["copy_vert_fwd",0,0],["copy_vert",0,0],["copy_vert_back",0,0],["repeat_op",0,3],["inc",0,0],["inc",1,0],["inc",2,0],["inc",3,0],["inc",4,0],["inc",5,0],["inc",6,0],["inc",7,0],["inc",8,0],["inc",9,0],["inc",10,0],["inc",11,0],["inc",12,0],["inc",13,0],["inc",14,0],["inc",15,0],["inc",16,0],["inc",17,0],["inc",18,0],["inc",19,0],["inc",20,0],["inc",21,0],["inc",22,0],["inc",23,0],["inc",24,0],["inc",25,0],["inc",26,0],["inc",27,0],["inc",28,0],["inc",29,0],["inc",30,0],["inc",31,0],["inc",32,0],["inc",33,0],["inc",34,0],["inc",35,0],["inc",36,0],["inc",37,0],["inc",38,0],["inc",39,0],["inc",40,0],["inc",41,0],["inc",42,0],["dec",0,0],["dec",1,0],["dec",2,0],["dec",3,0],["dec",4,0],["dec",5,0],["dec",6,0],["dec",7,0],["dec",8,0],["dec",9,0],["dec",10,0],["dec",11,0],["dec",12,0],["dec",13,0],["dec",14,0],["dec",15,0],["dec",16,0],["dec",17,0],["dec",18,0],["dec",19,0],["dec",20,0],["dec",21,0],["dec",22,0],["dec",23,0],["dec",24,0],["dec",25,0],["dec",26,0],["dec",27,0],["dec",28,0],["dec",29,0],["dec",30,0],["dec",31,0],["dec",32,0],["dec",33,0],["dec",34,0],["dec",35,0],["dec",36,0],["dec",37,0],["dec",38,0],["dec",39,0],["dec",40,0],["dec",41,0],["dec",42,0],</v>
+        <v>["raw",0,1],["raw",1,1],["raw",2,1],["copy_prev",0,0],["copy_vert_fwd",0,0],["copy_vert",0,0],["copy_vert_back",0,0],["repeat_op",0,3],["inc",0,0],["inc",1,0],["inc",2,0],["inc",3,0],["inc",4,0],["inc",5,0],["inc",6,0],["inc",7,0],["inc",8,0],["inc",9,0],["inc",10,0],["inc",11,0],["inc",12,0],["inc",13,0],["inc",14,0],["inc",15,0],["inc",16,0],["inc",17,0],["inc",18,0],["inc",19,0],["inc",20,0],["inc",21,0],["inc",22,0],["inc",23,0],["inc",24,0],["inc",25,0],["inc",26,0],["inc",27,0],["inc",28,0],["inc",29,0],["inc",30,0],["inc",31,0],["inc",32,0],["inc",33,0],["inc",34,0],["inc",35,0],["inc",36,0],["inc",37,0],["inc",38,0],["inc",39,0],["inc",40,0],["inc",41,0],["inc",42,0],["dec",0,0],["dec",1,0],["dec",2,0],["dec",3,0],["dec",4,0],["dec",5,0],["dec",6,0],["dec",7,0],["dec",8,0],["dec",9,0],["dec",10,0],["dec",11,0],["dec",12,0],["dec",13,0],["dec",14,0],["dec",15,0],["dec",16,0],["dec",17,0],["dec",18,0],["dec",19,0],["dec",20,0],["dec",21,0],["dec",22,0],["dec",23,0],["dec",24,0],["dec",25,0],["dec",26,0],["dec",27,0],["dec",28,0],["dec",29,0],["dec",30,0],["dec",31,0],["dec",32,0],["dec",33,0],["dec",34,0],["dec",35,0],["dec",36,0],["dec",37,0],["dec",38,0],["dec",39,0],["dec",40,0],["dec",41,0],["dec",42,0],</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -3377,11 +3377,11 @@
         <v>raw2</v>
       </c>
       <c r="F4" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H4" s="12" t="str">
         <f t="shared" si="1"/>
-        <v>["raw",2,0],</v>
+        <v>["raw",2,1],</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>